<commit_message>
Sixth neural network checkpoint: Latency testing finished
</commit_message>
<xml_diff>
--- a/documentation/figures/latencies.xlsx
+++ b/documentation/figures/latencies.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32914" windowHeight="14760"/>
   </bookViews>
   <sheets>
-    <sheet name="2400 (test)" sheetId="2" r:id="rId1"/>
-    <sheet name="2400 epochs" sheetId="1" r:id="rId2"/>
+    <sheet name="Main Page" sheetId="3" r:id="rId1"/>
+    <sheet name="Dont_use_this_data" sheetId="2" r:id="rId2"/>
+    <sheet name="2400 epochs" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
   <si>
     <t>Guess</t>
   </si>
@@ -186,14 +187,176 @@
     <t>D#M6</t>
   </si>
   <si>
-    <t>Numbers: Random.org</t>
+    <t>R2-B09</t>
+  </si>
+  <si>
+    <t>LATENCIES</t>
+  </si>
+  <si>
+    <t>System specs:</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>i7-5820K</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>Nvidia GTX 1070 (EVGA FTW2)</t>
+  </si>
+  <si>
+    <t>Disks</t>
+  </si>
+  <si>
+    <t>Sandisk SSD PLUS 120GB (MLC)</t>
+  </si>
+  <si>
+    <t>Samsung 850 EVO 256GB (MLC)</t>
+  </si>
+  <si>
+    <t>WD Black 1TB 7200RPM</t>
+  </si>
+  <si>
+    <t>revision</t>
+  </si>
+  <si>
+    <t>CMaug679M7sus4(9)</t>
+  </si>
+  <si>
+    <t>CMaug69M7sus2sus4(9)</t>
+  </si>
+  <si>
+    <t>Elapsed (NN only)</t>
+  </si>
+  <si>
+    <t>Elapsed (NN, ms)</t>
+  </si>
+  <si>
+    <t>CMaug69M7(9)</t>
+  </si>
+  <si>
+    <t>Caug79M7sus4(9)</t>
+  </si>
+  <si>
+    <t>CMaug679sus2sus4(9)</t>
+  </si>
+  <si>
+    <t>#NOTES</t>
+  </si>
+  <si>
+    <t>C#dim9</t>
+  </si>
+  <si>
+    <t>CMaug67M7(9)</t>
+  </si>
+  <si>
+    <t>CMaug679(9)</t>
+  </si>
+  <si>
+    <t>Caug69M7sus4(9)</t>
+  </si>
+  <si>
+    <t>Search time (ms)</t>
+  </si>
+  <si>
+    <t>Live perf thr (ms)</t>
+  </si>
+  <si>
+    <t>CMaug67M7sus2(9)</t>
+  </si>
+  <si>
+    <t>CM767M7sus4(9)</t>
+  </si>
+  <si>
+    <t>Caug67M7sus4(9)</t>
+  </si>
+  <si>
+    <t>Caug79M7sus2sus4(9)</t>
+  </si>
+  <si>
+    <t>Cmajaug69maj7sus4(9)</t>
+  </si>
+  <si>
+    <t>Caug679sus4(9)</t>
+  </si>
+  <si>
+    <t>CMaug79M7sus2sus4(9)</t>
+  </si>
+  <si>
+    <t>CMaug67M7sus4(9)</t>
+  </si>
+  <si>
+    <t>CMaug679sus4(9)</t>
+  </si>
+  <si>
+    <t>CMaug67sus4(9)</t>
+  </si>
+  <si>
+    <t>Caugdim69M7sus4(9)</t>
+  </si>
+  <si>
+    <t>Chords picked randomly</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>Summary measures</t>
+  </si>
+  <si>
+    <t>STDEV (Sample)</t>
+  </si>
+  <si>
+    <t>Samp Size</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>16GB Corsair Vengeance LPX 2400</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>1QT</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>3QT</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>1QT-MIN</t>
+  </si>
+  <si>
+    <t>MED-1QT</t>
+  </si>
+  <si>
+    <t>3QT-MED</t>
+  </si>
+  <si>
+    <t>MAX-3QT</t>
+  </si>
+  <si>
+    <t>Neural net</t>
+  </si>
+  <si>
+    <t>Neural net + Translator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,16 +390,41 @@
       <name val="HK Grotesk"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="HK Grotesk"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="HK Grotesk"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -244,22 +432,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFCCCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -269,6 +494,1124 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="HK Grotesk" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Neural network response times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="HK Grotesk" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="1"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$46:$G$46</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$46,'2400 epochs'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$47:$G$47</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$47,'2400 epochs'!$G$47)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.44000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1925000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2FDD-4D44-AB73-36E1ADD47A12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$46:$G$46</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$46,'2400 epochs'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$48:$G$48</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$48,'2400 epochs'!$G$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.9999999999999858E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2174999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2FDD-4D44-AB73-36E1ADD47A12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$46:$G$46</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$46,'2400 epochs'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$49:$G$49</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$49,'2400 epochs'!$G$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.20500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39500000000000046</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2FDD-4D44-AB73-36E1ADD47A12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="1"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$46:$G$46</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$46,'2400 epochs'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'2400 epochs'!$E$50:$G$50</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('2400 epochs'!$E$50,'2400 epochs'!$G$50)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84499999999999886</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2FDD-4D44-AB73-36E1ADD47A12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="617788816"/>
+        <c:axId val="617789144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="617788816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="HK Grotesk" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="617789144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="617789144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="HK Grotesk" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="617788816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="HK Grotesk" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>849086</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>106134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>557892</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558F2D9A-7B94-40AD-86CD-14AB2BFF06F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -568,10 +1911,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.23046875" style="1"/>
+    <col min="2" max="2" width="31.53515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3828125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.23046875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.299999999999997" x14ac:dyDescent="0.95">
+      <c r="B3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3046875" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -981,26 +2410,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3046875" defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.3046875" style="1"/>
     <col min="2" max="2" width="15.53515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3046875" style="1"/>
-    <col min="5" max="5" width="15.23046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.84375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.3046875" style="1"/>
+    <col min="3" max="3" width="25.69140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.23046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3046875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3046875" style="1"/>
+    <col min="7" max="7" width="15.23046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.84375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.53515625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="10.3046875" style="1"/>
+    <col min="12" max="12" width="23.765625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.3046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,268 +2445,1185 @@
         <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
+        <v>334</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="9">
+        <v>8.8000000000000003E-4</v>
+      </c>
+      <c r="E2" s="7">
+        <f>D2*1000</f>
+        <v>0.88</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.5100000000000001E-3</v>
+      </c>
+      <c r="G2" s="8">
+        <f>F2*1000</f>
+        <v>1.51</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <f>1000*(F2-D2)</f>
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
+        <v>388</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E3" s="7">
+        <f>D3*1000</f>
+        <v>1.3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.1199999999999999E-3</v>
+      </c>
+      <c r="G3" s="8">
+        <f>F3*1000</f>
+        <v>2.12</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
+        <f>1000*(F3-D3)</f>
+        <v>0.82</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="2">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1.3699999999999999E-3</v>
+      </c>
+      <c r="E4" s="7">
+        <f>D4*1000</f>
+        <v>1.3699999999999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.1900000000000001E-3</v>
+      </c>
+      <c r="G4" s="8">
+        <f>F4*1000</f>
+        <v>2.19</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <f>1000*(F4-D4)</f>
+        <v>0.82000000000000017</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3">
+      <c r="M4" s="3">
         <v>2400</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
-        <v>77</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
+        <v>150</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2.16E-3</v>
+      </c>
+      <c r="E5" s="7">
+        <f>D5*1000</f>
+        <v>2.16</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.0500000000000002E-3</v>
+      </c>
+      <c r="G5" s="8">
+        <f>F5*1000</f>
+        <v>3.0500000000000003</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <f>1000*(F5-D5)</f>
+        <v>0.89000000000000012</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
         <v>82</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <v>423</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
-        <v>368</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
-        <v>217</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1.47E-3</v>
+      </c>
+      <c r="E6" s="7">
+        <f>D6*1000</f>
+        <v>1.47</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.3700000000000001E-3</v>
+      </c>
+      <c r="G6" s="8">
+        <f>F6*1000</f>
+        <v>2.37</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <f>1000*(F6-D6)</f>
+        <v>0.90000000000000024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>247</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1.48E-3</v>
+      </c>
+      <c r="E7" s="7">
+        <f>D7*1000</f>
+        <v>1.48</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="G7" s="8">
+        <f>F7*1000</f>
+        <v>2.4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1">
+        <f>1000*(F7-D7)</f>
+        <v>0.91999999999999982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>302</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2.0100000000000001E-3</v>
+      </c>
+      <c r="E8" s="7">
+        <f>D8*1000</f>
+        <v>2.0100000000000002</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.96E-3</v>
+      </c>
+      <c r="G8" s="8">
+        <f>F8*1000</f>
+        <v>2.96</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1">
+        <f>1000*(F8-D8)</f>
+        <v>0.94999999999999984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
-        <v>44</v>
+        <v>305</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E9" s="7">
+        <f>D9*1000</f>
+        <v>1.3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.2499999999999998E-3</v>
+      </c>
+      <c r="G9" s="8">
+        <f>F9*1000</f>
+        <v>2.25</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <f>1000*(F9-D9)</f>
+        <v>0.94999999999999984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
-        <v>420</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1.99E-3</v>
+      </c>
+      <c r="E10" s="7">
+        <f>D10*1000</f>
+        <v>1.99</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.98E-3</v>
+      </c>
+      <c r="G10" s="8">
+        <f>F10*1000</f>
+        <v>2.98</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1">
+        <f>1000*(F10-D10)</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2.1900000000000001E-3</v>
+      </c>
+      <c r="E11" s="7">
+        <f>D11*1000</f>
+        <v>2.19</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="G11" s="8">
+        <f>F11*1000</f>
+        <v>3.18</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1">
+        <f>1000*(F11-D11)</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="2">
-        <v>427</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1.6199999999999999E-3</v>
+      </c>
+      <c r="E12" s="7">
+        <f>D12*1000</f>
+        <v>1.6199999999999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.63E-3</v>
+      </c>
+      <c r="G12" s="8">
+        <f>F12*1000</f>
+        <v>2.63</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1">
+        <f>1000*(F12-D12)</f>
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>424</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="C13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="E13" s="7">
+        <f>D13*1000</f>
+        <v>1.52</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F13*1000</f>
+        <v>2.7</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1">
+        <f>1000*(F13-D13)</f>
+        <v>1.1800000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
+        <v>247</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1.42E-3</v>
+      </c>
+      <c r="E14" s="7">
+        <f>D14*1000</f>
+        <v>1.42</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.7100000000000002E-3</v>
+      </c>
+      <c r="G14" s="8">
+        <f>F14*1000</f>
+        <v>2.71</v>
+      </c>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1">
+        <f>1000*(F14-D14)</f>
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
+        <v>438</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1.32E-3</v>
+      </c>
+      <c r="E15" s="7">
+        <f>D15*1000</f>
+        <v>1.32</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2.7399999999999998E-3</v>
+      </c>
+      <c r="G15" s="8">
+        <f>F15*1000</f>
+        <v>2.7399999999999998</v>
+      </c>
+      <c r="H15" s="1">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1">
+        <f>1000*(F15-D15)</f>
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="2">
+        <v>217</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1.32E-3</v>
+      </c>
+      <c r="E16" s="7">
+        <f>D16*1000</f>
+        <v>1.32</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.7699999999999999E-3</v>
+      </c>
+      <c r="G16" s="8">
+        <f>F16*1000</f>
+        <v>2.77</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1">
+        <f>1000*(F16-D16)</f>
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="2">
+        <v>368</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1.57E-3</v>
+      </c>
+      <c r="E17" s="7">
+        <f>D17*1000</f>
+        <v>1.57</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.0599999999999998E-3</v>
+      </c>
+      <c r="G17" s="8">
+        <f>F17*1000</f>
+        <v>3.0599999999999996</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1">
+        <f>1000*(F17-D17)</f>
+        <v>1.4899999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
+        <v>145</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1.2899999999999999E-3</v>
+      </c>
+      <c r="E18" s="7">
+        <f>D18*1000</f>
+        <v>1.2899999999999998</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2.8E-3</v>
+      </c>
+      <c r="G18" s="8">
+        <f>F18*1000</f>
+        <v>2.8</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <f>1000*(F18-D18)</f>
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
+        <v>405</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1.31E-3</v>
+      </c>
+      <c r="E19" s="7">
+        <f>D19*1000</f>
+        <v>1.31</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2.8300000000000001E-3</v>
+      </c>
+      <c r="G19" s="8">
+        <f>F19*1000</f>
+        <v>2.83</v>
+      </c>
+      <c r="H19" s="1">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1">
+        <f>1000*(F19-D19)</f>
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="2">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1.2700000000000001E-3</v>
+      </c>
+      <c r="E20" s="7">
+        <f>D20*1000</f>
+        <v>1.27</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2.8600000000000001E-3</v>
+      </c>
+      <c r="G20" s="8">
+        <f>F20*1000</f>
+        <v>2.8600000000000003</v>
+      </c>
+      <c r="H20" s="1">
+        <v>5</v>
+      </c>
+      <c r="I20" s="1">
+        <f>1000*(F20-D20)</f>
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="2">
+        <v>68</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1.2800000000000001E-3</v>
+      </c>
+      <c r="E21" s="7">
+        <f>D21*1000</f>
+        <v>1.28</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.8800000000000002E-3</v>
+      </c>
+      <c r="G21" s="8">
+        <f>F21*1000</f>
+        <v>2.8800000000000003</v>
+      </c>
+      <c r="H21" s="1">
+        <v>6</v>
+      </c>
+      <c r="I21" s="1">
+        <f>1000*(F21-D21)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="2">
         <v>182</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="2">
-        <v>305</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="2">
-        <v>334</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="2">
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E22" s="7">
+        <f>D22*1000</f>
+        <v>1.6</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3.3400000000000001E-3</v>
+      </c>
+      <c r="G22" s="8">
+        <f>F22*1000</f>
+        <v>3.3400000000000003</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1">
+        <f>1000*(F22-D22)</f>
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="2">
+        <v>204</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1.33E-3</v>
+      </c>
+      <c r="E23" s="7">
+        <f>D23*1000</f>
+        <v>1.33</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3.13E-3</v>
+      </c>
+      <c r="G23" s="8">
+        <f>F23*1000</f>
+        <v>3.13</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5</v>
+      </c>
+      <c r="I23" s="1">
+        <f>1000*(F23-D23)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="2">
+        <v>227</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="9">
+        <v>2.0300000000000001E-3</v>
+      </c>
+      <c r="E24" s="7">
+        <f>D24*1000</f>
+        <v>2.0300000000000002</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3.9100000000000003E-3</v>
+      </c>
+      <c r="G24" s="8">
+        <f>F24*1000</f>
+        <v>3.91</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1">
+        <f>1000*(F24-D24)</f>
+        <v>1.8800000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25" s="2">
+        <v>272</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="9">
+        <v>1.32E-3</v>
+      </c>
+      <c r="E25" s="7">
+        <f>D25*1000</f>
+        <v>1.32</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3.2399999999999998E-3</v>
+      </c>
+      <c r="G25" s="8">
+        <f>F25*1000</f>
+        <v>3.2399999999999998</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4</v>
+      </c>
+      <c r="I25" s="1">
+        <f>1000*(F25-D25)</f>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A26" s="2">
+        <v>357</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1.32E-3</v>
+      </c>
+      <c r="E26" s="7">
+        <f>D26*1000</f>
+        <v>1.32</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3.3400000000000001E-3</v>
+      </c>
+      <c r="G26" s="8">
+        <f>F26*1000</f>
+        <v>3.3400000000000003</v>
+      </c>
+      <c r="H26" s="1">
+        <v>5</v>
+      </c>
+      <c r="I26" s="1">
+        <f>1000*(F26-D26)</f>
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
+        <v>420</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1.6199999999999999E-3</v>
+      </c>
+      <c r="E27" s="7">
+        <f>D27*1000</f>
+        <v>1.6199999999999999</v>
+      </c>
+      <c r="F27" s="1">
+        <v>3.7200000000000002E-3</v>
+      </c>
+      <c r="G27" s="8">
+        <f>F27*1000</f>
+        <v>3.72</v>
+      </c>
+      <c r="H27" s="1">
+        <v>4</v>
+      </c>
+      <c r="I27" s="1">
+        <f>1000*(F27-D27)</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
+        <v>409</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="9">
+        <v>2.0500000000000002E-3</v>
+      </c>
+      <c r="E28" s="7">
+        <f>D28*1000</f>
+        <v>2.0500000000000003</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="G28" s="8">
+        <f>F28*1000</f>
+        <v>4.1599999999999993</v>
+      </c>
+      <c r="H28" s="1">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1">
+        <f>1000*(F28-D28)</f>
+        <v>2.1099999999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
+        <v>423</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1.5900000000000001E-3</v>
+      </c>
+      <c r="E29" s="7">
+        <f>D29*1000</f>
+        <v>1.59</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3.7200000000000002E-3</v>
+      </c>
+      <c r="G29" s="8">
+        <f>F29*1000</f>
+        <v>3.72</v>
+      </c>
+      <c r="H29" s="1">
+        <v>4</v>
+      </c>
+      <c r="I29" s="1">
+        <f>1000*(F29-D29)</f>
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A30" s="2">
+        <v>427</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="9">
+        <v>1.3500000000000001E-3</v>
+      </c>
+      <c r="E30" s="7">
+        <f>D30*1000</f>
+        <v>1.35</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3.48E-3</v>
+      </c>
+      <c r="G30" s="8">
+        <f>F30*1000</f>
+        <v>3.48</v>
+      </c>
+      <c r="H30" s="1">
+        <v>5</v>
+      </c>
+      <c r="I30" s="1">
+        <f>1000*(F30-D30)</f>
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A31" s="2">
         <v>211</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" s="2">
-        <v>438</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" s="2">
-        <v>150</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" s="2">
+      <c r="C31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="9">
+        <v>1.4E-3</v>
+      </c>
+      <c r="E31" s="7">
+        <f>D31*1000</f>
+        <v>1.4</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3.6099999999999999E-3</v>
+      </c>
+      <c r="G31" s="8">
+        <f>F31*1000</f>
+        <v>3.61</v>
+      </c>
+      <c r="H31" s="1">
         <v>6</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" s="2">
-        <v>388</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" s="2">
-        <v>357</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="2">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="2">
-        <v>305</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" s="2">
-        <v>405</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" s="2">
-        <v>68</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" s="2">
-        <v>204</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" s="2">
-        <v>272</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="2">
-        <v>409</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" s="2">
-        <v>227</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" s="2">
-        <v>145</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B33" s="1" t="s">
-        <v>53</v>
+      <c r="I31" s="1">
+        <f>1000*(F31-D31)</f>
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="11">
+        <f>AVERAGE(E2:E31)</f>
+        <v>1.5226666666666666</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="12">
+        <f>AVERAGE(G2:G31)</f>
+        <v>2.9546666666666668</v>
+      </c>
+      <c r="I36" s="2">
+        <f>AVERAGE(I2:I31)</f>
+        <v>1.4320000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="11">
+        <f>_xlfn.STDEV.S(E2:E31)</f>
+        <v>0.31587790453704268</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="12">
+        <f>_xlfn.STDEV.S(G2:G31)</f>
+        <v>0.57541429352719786</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="11">
+        <v>30</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="1">
+        <f>MIN(E2:E31)</f>
+        <v>0.88</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" ref="F40:G40" si="0">MIN(G2:G31)</f>
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 1)</f>
+        <v>1.32</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" ref="F41:G41" si="1">_xlfn.QUARTILE.INC(G2:G31, 1)</f>
+        <v>2.7025000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 2)</f>
+        <v>1.41</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" ref="F42:G42" si="2">_xlfn.QUARTILE.INC(G2:G31, 2)</f>
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 3)</f>
+        <v>1.615</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" ref="F43:G43" si="3">_xlfn.QUARTILE.INC(G2:G31, 3)</f>
+        <v>3.3150000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C44" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="1">
+        <f>MAX(E2:E31)</f>
+        <v>2.19</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" ref="F44:G44" si="4">MAX(G2:G31)</f>
+        <v>4.1599999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="E46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C47" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="1">
+        <f>E41-E40</f>
+        <v>0.44000000000000006</v>
+      </c>
+      <c r="G47" s="1">
+        <f>G41-G40</f>
+        <v>1.1925000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C48" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" s="1">
+        <f>E42-E41</f>
+        <v>8.9999999999999858E-2</v>
+      </c>
+      <c r="G48" s="1">
+        <f>G42-G41</f>
+        <v>0.2174999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C49" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" s="1">
+        <f>E43-E42</f>
+        <v>0.20500000000000007</v>
+      </c>
+      <c r="G49" s="1">
+        <f>G43-G42</f>
+        <v>0.39500000000000046</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="1">
+        <f>E44-E43</f>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="G50" s="1">
+        <f>G44-G43</f>
+        <v>0.84499999999999886</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I31">
+    <sortCondition ref="I2:I31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected STDEV.S in latencies file
</commit_message>
<xml_diff>
--- a/documentation/figures/latencies.xlsx
+++ b/documentation/figures/latencies.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="1" state="visible" r:id="rId2"/>
@@ -860,7 +860,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.0899999999999999</c:v>
+                  <c:v>0.0899999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.2175</c:v>
@@ -970,7 +970,7 @@
                   <c:v>0.575</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.844999999999999</c:v>
+                  <c:v>0.845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -978,11 +978,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="25396968"/>
-        <c:axId val="65775026"/>
+        <c:axId val="44806562"/>
+        <c:axId val="67673302"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="25396968"/>
+        <c:axId val="44806562"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,14 +1018,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65775026"/>
+        <c:crossAx val="67673302"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65775026"/>
+        <c:axId val="67673302"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1068,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25396968"/>
+        <c:crossAx val="44806562"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1107,9 +1107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>71280</xdr:rowOff>
+      <xdr:rowOff>70920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1117,8 +1117,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2961360" y="9324720"/>
-        <a:ext cx="6309360" cy="3715560"/>
+        <a:off x="2984040" y="9324720"/>
+        <a:ext cx="6423480" cy="3715200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1144,10 +1144,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.6122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.9540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.1530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1251,13 +1251,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.6938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,24 +1673,24 @@
   </sheetPr>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.4948979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.5816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="10.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.780612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="17.1734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.984693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.8418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="10.6938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2929,9 +2929,9 @@
       <c r="C37" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="14" t="e">
-        <f aca="false">k11s</f>
-        <v>#NAME?</v>
+      <c r="E37" s="14" t="n">
+        <f aca="false">_xlfn.STDEV.S(E2:E31)</f>
+        <v>0.315877904537042</v>
       </c>
       <c r="F37" s="13"/>
       <c r="G37" s="15" t="n">
@@ -3137,8 +3137,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,14 +3314,14 @@
   </sheetPr>
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Finished documentation for A.N13
</commit_message>
<xml_diff>
--- a/documentation/figures/latencies.xlsx
+++ b/documentation/figures/latencies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="129">
   <si>
     <t xml:space="preserve">R2-B09</t>
   </si>
@@ -713,7 +713,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -978,11 +978,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="44806562"/>
-        <c:axId val="67673302"/>
+        <c:axId val="10204729"/>
+        <c:axId val="95714024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44806562"/>
+        <c:axId val="10204729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,14 +1018,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67673302"/>
+        <c:crossAx val="95714024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67673302"/>
+        <c:axId val="95714024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1068,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44806562"/>
+        <c:crossAx val="10204729"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1107,9 +1107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>65520</xdr:colOff>
+      <xdr:colOff>65160</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>70920</xdr:rowOff>
+      <xdr:rowOff>70560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1117,8 +1117,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2984040" y="9324720"/>
-        <a:ext cx="6423480" cy="3715200"/>
+        <a:off x="3007080" y="9324720"/>
+        <a:ext cx="6537240" cy="3714840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1139,15 +1139,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="K25:L40 D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.1530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.6938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="9.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,7 +1170,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,18 +1246,18 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K25:L40 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.4132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,24 +1673,24 @@
   </sheetPr>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.780612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="17.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.984693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.8418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.4132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.2142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="17.4948979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.4132653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.1683673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,13 +3132,13 @@
   <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="K25:L40 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.7704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3312,170 +3312,264 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="K25:L40 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.7704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7" t="n">
         <v>1.51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7" t="n">
         <v>2.12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="7" t="n">
         <v>2.19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="7" t="n">
         <v>3.05</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="7" t="n">
         <v>2.37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="7" t="n">
         <v>2.4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+      <c r="A8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="7" t="n">
         <v>2.96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+      <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="7" t="n">
         <v>2.25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+      <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="7" t="n">
         <v>2.98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+      <c r="A11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="7" t="n">
         <v>3.18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+      <c r="A12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="7" t="n">
         <v>2.63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="7" t="n">
         <v>2.7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="7" t="n">
         <v>2.71</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="n">
         <v>2.74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
+      <c r="A16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="7" t="n">
         <v>2.77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
+      <c r="A17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="7" t="n">
         <v>3.06</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+      <c r="A18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="7" t="n">
         <v>2.8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+      <c r="A19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="7" t="n">
         <v>2.83</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+      <c r="A20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="7" t="n">
         <v>2.86</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+      <c r="A21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="7" t="n">
         <v>2.88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+      <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="7" t="n">
         <v>3.34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+      <c r="A23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="7" t="n">
         <v>3.13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+      <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="7" t="n">
         <v>3.91</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+      <c r="A25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="7" t="n">
         <v>3.24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+      <c r="A26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="7" t="n">
         <v>3.34</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="n">
+      <c r="A27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="7" t="n">
         <v>3.72</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="n">
+      <c r="A28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="7" t="n">
         <v>4.16</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="n">
+      <c r="A29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="7" t="n">
         <v>3.72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="n">
+      <c r="A30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="7" t="n">
         <v>3.48</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
+      <c r="A31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="7" t="n">
         <v>3.61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel latencies finished; py files updated with latency testing
</commit_message>
<xml_diff>
--- a/documentation/figures/latencies.xlsx
+++ b/documentation/figures/latencies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joachim\Documents\PSHS 2019\5\R2_B09_Chord_Identification\documentation\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\PSHS 2019\5\R2_B09_Chord_Identification\documentation\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FF3C86-CD64-4024-BC9F-A14E76CDFD3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C143FEFB-70CF-4C97-B088-C1466558AE78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="989" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,11 @@
     <sheet name="2400 epochs" sheetId="3" r:id="rId3"/>
     <sheet name="NNtime" sheetId="4" r:id="rId4"/>
     <sheet name="Totaltime" sheetId="5" r:id="rId5"/>
-    <sheet name="6_NN2_4000-epochs" sheetId="6" r:id="rId6"/>
+    <sheet name="6_NN2_4000" sheetId="7" r:id="rId6"/>
+    <sheet name="A" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="182">
   <si>
     <t>R2-B09</t>
   </si>
@@ -422,6 +418,165 @@
   </si>
   <si>
     <t>Total time</t>
+  </si>
+  <si>
+    <t>Bmin</t>
+  </si>
+  <si>
+    <t>G#o7</t>
+  </si>
+  <si>
+    <t>GmM7(9)</t>
+  </si>
+  <si>
+    <t>A#M7sus2</t>
+  </si>
+  <si>
+    <t>Caug7</t>
+  </si>
+  <si>
+    <t>F#sus4</t>
+  </si>
+  <si>
+    <t>Em7</t>
+  </si>
+  <si>
+    <t>Gdim7</t>
+  </si>
+  <si>
+    <t>G#m7sus2</t>
+  </si>
+  <si>
+    <t>G#dim</t>
+  </si>
+  <si>
+    <t>Faug11</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>A#11</t>
+  </si>
+  <si>
+    <t>Aaug9</t>
+  </si>
+  <si>
+    <t>G#M9sus2</t>
+  </si>
+  <si>
+    <t>D#M9</t>
+  </si>
+  <si>
+    <t>BM9sus2</t>
+  </si>
+  <si>
+    <t>D#m6(9)</t>
+  </si>
+  <si>
+    <t>F#min</t>
+  </si>
+  <si>
+    <t>Faug</t>
+  </si>
+  <si>
+    <t>Do7</t>
+  </si>
+  <si>
+    <t>Adim7</t>
+  </si>
+  <si>
+    <t>C#M11</t>
+  </si>
+  <si>
+    <t>G#M7</t>
+  </si>
+  <si>
+    <t>F#M7sus4</t>
+  </si>
+  <si>
+    <t>G#9sus4</t>
+  </si>
+  <si>
+    <t>Esus2</t>
+  </si>
+  <si>
+    <t>D#aug7</t>
+  </si>
+  <si>
+    <t>G#dim9</t>
+  </si>
+  <si>
+    <t>CM9sus4</t>
+  </si>
+  <si>
+    <t>EM6(9)</t>
+  </si>
+  <si>
+    <t>DM7sus2</t>
+  </si>
+  <si>
+    <t>F#mM7</t>
+  </si>
+  <si>
+    <t>Edim9</t>
+  </si>
+  <si>
+    <t>Em6(9)</t>
+  </si>
+  <si>
+    <t>C#m9</t>
+  </si>
+  <si>
+    <t>A#9sus4</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>DmM7(9)</t>
+  </si>
+  <si>
+    <t>A7sus2</t>
+  </si>
+  <si>
+    <t>F#m7</t>
+  </si>
+  <si>
+    <t>G#dim7</t>
+  </si>
+  <si>
+    <t>F#M6</t>
+  </si>
+  <si>
+    <t>Dmaj</t>
+  </si>
+  <si>
+    <t>F#11sus2</t>
+  </si>
+  <si>
+    <t>G7sus4</t>
+  </si>
+  <si>
+    <t>Gdim</t>
+  </si>
+  <si>
+    <t>Gm6</t>
+  </si>
+  <si>
+    <t>EM7</t>
+  </si>
+  <si>
+    <t>G#M11</t>
+  </si>
+  <si>
+    <t>Csus2</t>
+  </si>
+  <si>
+    <t>H0: m &gt;= 40</t>
+  </si>
+  <si>
+    <t>HA: m &lt; 40</t>
   </si>
 </sst>
 </file>
@@ -688,7 +843,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1400" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1136,6 +1291,488 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:rPr>
+              <a:t>Neural network response times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_4000'!$E$46,'6_NN2_4000'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_4000'!$E$47,'6_NN2_4000'!$G$47)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.21250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43249999999999988</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DBE5-44DC-BA69-F0571F1F817B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_4000'!$E$46,'6_NN2_4000'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_4000'!$E$48,'6_NN2_4000'!$G$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.7499999999999969E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5000000000000622E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DBE5-44DC-BA69-F0571F1F817B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="A5A5A5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_4000'!$E$46,'6_NN2_4000'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_4000'!$E$49,'6_NN2_4000'!$G$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>4.7499999999999987E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0925000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DBE5-44DC-BA69-F0571F1F817B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_4000'!$E$46,'6_NN2_4000'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_4000'!$E$50,'6_NN2_4000'!$G$50)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.40250000000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9074999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DBE5-44DC-BA69-F0571F1F817B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="10204729"/>
+        <c:axId val="95714024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="10204729"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95714024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95714024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10204729"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1161,6 +1798,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1086840</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342746</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56469778-E25B-4E54-8527-71879B61B600}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1480,20 +2160,20 @@
       <selection activeCell="D3" activeCellId="1" sqref="K25:L40 D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" style="1"/>
-    <col min="2" max="2" width="33.6640625" style="1"/>
-    <col min="3" max="3" width="17.5546875" style="1"/>
-    <col min="4" max="1025" width="9.77734375" style="1"/>
+    <col min="1" max="1" width="9.765625" style="1"/>
+    <col min="2" max="2" width="33.69140625" style="1"/>
+    <col min="3" max="3" width="17.53515625" style="1"/>
+    <col min="4" max="1025" width="9.765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1"/>
       <c r="B1"/>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1502,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34.200000000000003" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:4" ht="34.299999999999997" x14ac:dyDescent="0.95">
       <c r="A3"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -1511,17 +2191,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1529,7 +2209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1537,7 +2217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1545,19 +2225,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1579,18 +2259,18 @@
       <selection activeCellId="1" sqref="K25:L40 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="1"/>
-    <col min="2" max="2" width="16.44140625" style="1"/>
-    <col min="3" max="3" width="17.21875" style="1"/>
-    <col min="4" max="4" width="10.77734375" style="1"/>
-    <col min="5" max="5" width="16.109375" style="1"/>
-    <col min="6" max="6" width="17.88671875" style="1"/>
-    <col min="7" max="1025" width="10.77734375" style="1"/>
+    <col min="1" max="1" width="10.765625" style="1"/>
+    <col min="2" max="2" width="16.4609375" style="1"/>
+    <col min="3" max="3" width="17.23046875" style="1"/>
+    <col min="4" max="4" width="10.765625" style="1"/>
+    <col min="5" max="5" width="16.07421875" style="1"/>
+    <col min="6" max="6" width="17.84375" style="1"/>
+    <col min="7" max="1025" width="10.765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1616,7 +2296,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1637,7 +2317,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1656,7 +2336,7 @@
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1675,7 +2355,7 @@
       </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1694,7 +2374,7 @@
       </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1713,7 +2393,7 @@
       </c>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1732,7 +2412,7 @@
       </c>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1753,7 +2433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1771,7 +2451,7 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1789,7 +2469,7 @@
         <v>1.5299999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1807,7 +2487,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1825,7 +2505,7 @@
         <v>1.2899999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1843,7 +2523,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1861,7 +2541,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1879,7 +2559,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1897,7 +2577,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1915,72 +2595,72 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2000,26 +2680,26 @@
   <dimension ref="A1:AMK50"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="1"/>
-    <col min="2" max="2" width="16.44140625" style="1"/>
-    <col min="3" max="3" width="27.21875" style="1"/>
-    <col min="4" max="5" width="17.44140625" style="1"/>
-    <col min="6" max="6" width="10.77734375" style="1"/>
-    <col min="7" max="7" width="16.21875" style="1"/>
-    <col min="8" max="8" width="17.88671875" style="1"/>
-    <col min="9" max="9" width="16.44140625" style="1"/>
-    <col min="10" max="10" width="10.77734375" style="1"/>
-    <col min="11" max="11" width="21.21875" style="1"/>
-    <col min="12" max="12" width="25.33203125" style="1"/>
-    <col min="13" max="1025" width="10.77734375" style="1"/>
+    <col min="1" max="1" width="10.765625" style="1"/>
+    <col min="2" max="2" width="16.4609375" style="1"/>
+    <col min="3" max="3" width="27.23046875" style="1"/>
+    <col min="4" max="5" width="17.4609375" style="1"/>
+    <col min="6" max="6" width="10.765625" style="1"/>
+    <col min="7" max="7" width="16.23046875" style="1"/>
+    <col min="8" max="8" width="17.84375" style="1"/>
+    <col min="9" max="9" width="16.4609375" style="1"/>
+    <col min="10" max="10" width="10.765625" style="1"/>
+    <col min="11" max="11" width="21.23046875" style="1"/>
+    <col min="12" max="12" width="25.3046875" style="1"/>
+    <col min="13" max="1025" width="10.765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -2050,7 +2730,7 @@
       <c r="K1"/>
       <c r="L1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>334</v>
       </c>
@@ -2084,7 +2764,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>388</v>
       </c>
@@ -2120,7 +2800,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>77</v>
       </c>
@@ -2156,7 +2836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>150</v>
       </c>
@@ -2192,7 +2872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>82</v>
       </c>
@@ -2226,7 +2906,7 @@
       <c r="K6"/>
       <c r="L6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>44</v>
       </c>
@@ -2264,7 +2944,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>302</v>
       </c>
@@ -2302,7 +2982,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>305</v>
       </c>
@@ -2338,7 +3018,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -2376,7 +3056,7 @@
         <v>1.5226666666666699</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>4</v>
       </c>
@@ -2415,7 +3095,7 @@
         <v>0.31587790453704268</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>25</v>
       </c>
@@ -2453,7 +3133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>424</v>
       </c>
@@ -2491,7 +3171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>247</v>
       </c>
@@ -2530,7 +3210,7 @@
         <v>5.7671151244133911E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>438</v>
       </c>
@@ -2568,7 +3248,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>217</v>
       </c>
@@ -2606,7 +3286,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>368</v>
       </c>
@@ -2645,7 +3325,7 @@
         <v>-31.475227313944458</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>145</v>
       </c>
@@ -2684,7 +3364,7 @@
         <v>2.843196868216149E-24</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>405</v>
       </c>
@@ -2723,7 +3403,7 @@
         <v>-1.6991270265334986</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>58</v>
       </c>
@@ -2757,7 +3437,7 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>68</v>
       </c>
@@ -2795,7 +3475,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>182</v>
       </c>
@@ -2833,7 +3513,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>204</v>
       </c>
@@ -2867,7 +3547,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>227</v>
       </c>
@@ -2901,7 +3581,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>272</v>
       </c>
@@ -2939,7 +3619,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>357</v>
       </c>
@@ -2977,7 +3657,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>420</v>
       </c>
@@ -3013,7 +3693,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>409</v>
       </c>
@@ -3052,7 +3732,7 @@
         <v>2.9546666666666668</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>423</v>
       </c>
@@ -3091,7 +3771,7 @@
         <v>0.57541429352719786</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>427</v>
       </c>
@@ -3129,7 +3809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>211</v>
       </c>
@@ -3167,7 +3847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B32"/>
       <c r="C32"/>
       <c r="E32"/>
@@ -3182,7 +3862,7 @@
         <v>0.10505579615858172</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B33"/>
       <c r="C33"/>
       <c r="E33"/>
@@ -3196,7 +3876,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B34" s="2"/>
       <c r="C34"/>
       <c r="E34"/>
@@ -3210,7 +3890,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C35" s="1" t="s">
         <v>111</v>
       </c>
@@ -3226,7 +3906,7 @@
         <v>-17.196208566851876</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C36" s="2" t="s">
         <v>112</v>
       </c>
@@ -3251,7 +3931,7 @@
         <v>4.7098882080482392E-17</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C37" s="2" t="s">
         <v>113</v>
       </c>
@@ -3272,7 +3952,7 @@
         <v>-1.6991270265334986</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C38" s="2" t="s">
         <v>114</v>
       </c>
@@ -3286,7 +3966,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C39"/>
       <c r="E39"/>
       <c r="G39"/>
@@ -3297,7 +3977,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C40" s="2" t="s">
         <v>115</v>
       </c>
@@ -3316,7 +3996,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C41" s="2" t="s">
         <v>116</v>
       </c>
@@ -3330,7 +4010,7 @@
       </c>
       <c r="L41"/>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C42" s="2" t="s">
         <v>117</v>
       </c>
@@ -3346,7 +4026,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C43" s="2" t="s">
         <v>119</v>
       </c>
@@ -3359,7 +4039,7 @@
         <v>3.3150000000000004</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C44" s="2" t="s">
         <v>120</v>
       </c>
@@ -3372,12 +4052,12 @@
         <v>4.1599999999999993</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C45"/>
       <c r="E45"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C46"/>
       <c r="E46" s="2" t="s">
         <v>121</v>
@@ -3386,7 +4066,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C47" s="2" t="s">
         <v>123</v>
       </c>
@@ -3399,7 +4079,7 @@
         <v>1.1925000000000001</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.45">
       <c r="C48" s="2" t="s">
         <v>124</v>
       </c>
@@ -3412,7 +4092,7 @@
         <v>0.2174999999999998</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C49" s="2" t="s">
         <v>125</v>
       </c>
@@ -3425,7 +4105,7 @@
         <v>0.39500000000000046</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C50" s="2" t="s">
         <v>126</v>
       </c>
@@ -3453,163 +4133,163 @@
       <selection activeCell="C1" activeCellId="1" sqref="K25:L40 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.33203125"/>
-    <col min="2" max="1025" width="11.77734375"/>
+    <col min="1" max="1" width="18.3046875"/>
+    <col min="2" max="1025" width="11.765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A2" s="6">
         <v>0.88</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>1.37</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <v>2.16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <v>1.47</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <v>1.48</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
         <v>1.3</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <v>1.99</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
         <v>2.19</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>1.62</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <v>1.52</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>1.42</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <v>1.32</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <v>1.32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <v>1.57</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <v>1.29</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>1.31</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <v>1.27</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
         <v>1.28</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <v>1.6</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <v>1.33</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <v>1.32</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <v>1.32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
         <v>1.62</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
         <v>1.59</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <v>1.35</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="15" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <v>1.4</v>
       </c>
@@ -3632,14 +4312,14 @@
       <selection activeCell="C6" activeCellId="1" sqref="K25:L40 C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.77734375"/>
-    <col min="2" max="2" width="16.6640625"/>
-    <col min="3" max="1025" width="11.77734375"/>
+    <col min="1" max="1" width="15.765625"/>
+    <col min="2" max="2" width="16.69140625"/>
+    <col min="3" max="1025" width="11.765625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -3647,7 +4327,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -3655,7 +4335,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -3663,7 +4343,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -3671,7 +4351,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -3679,7 +4359,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -3687,7 +4367,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -3695,7 +4375,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>57</v>
       </c>
@@ -3703,7 +4383,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
@@ -3711,7 +4391,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -3719,7 +4399,7 @@
         <v>2.98</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -3727,7 +4407,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>68</v>
       </c>
@@ -3735,7 +4415,7 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
@@ -3743,7 +4423,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>74</v>
       </c>
@@ -3751,7 +4431,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>77</v>
       </c>
@@ -3759,7 +4439,7 @@
         <v>2.74</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>79</v>
       </c>
@@ -3767,7 +4447,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -3775,7 +4455,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
@@ -3783,7 +4463,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -3791,7 +4471,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>91</v>
       </c>
@@ -3799,7 +4479,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -3807,7 +4487,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>95</v>
       </c>
@@ -3815,7 +4495,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>97</v>
       </c>
@@ -3823,7 +4503,7 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>99</v>
       </c>
@@ -3831,7 +4511,7 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -3839,7 +4519,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>102</v>
       </c>
@@ -3847,7 +4527,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>103</v>
       </c>
@@ -3855,7 +4535,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
@@ -3863,7 +4543,7 @@
         <v>4.16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>106</v>
       </c>
@@ -3871,7 +4551,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>108</v>
       </c>
@@ -3879,7 +4559,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>110</v>
       </c>
@@ -3898,12 +4578,1381 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96F28FD-0BBF-4F5B-9859-054629604D05}">
+  <dimension ref="A1:AMK50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.23046875" style="1"/>
+    <col min="2" max="2" width="15.84375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3046875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.53515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.61328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.23046875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.69140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23046875" style="1"/>
+    <col min="11" max="11" width="17.3046875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.61328125" style="1" customWidth="1"/>
+    <col min="13" max="1025" width="9.23046875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1"/>
+      <c r="L1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
+        <v>409</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1.2199999999999999E-3</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:E31" si="0">D2*1000</f>
+        <v>1.22</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.8699999999999999E-3</v>
+      </c>
+      <c r="G2" s="7">
+        <f t="shared" ref="G2:G31" si="1">F2*1000</f>
+        <v>1.8699999999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I31" si="2">1000*(F2-D2)</f>
+        <v>0.65</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
+        <v>308</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8.8999999999999995E-4</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" si="1"/>
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="2"/>
+        <v>5.01</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="2">
+        <v>329</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="5">
+        <v>9.3999999999999997E-4</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.7399999999999998E-3</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="1"/>
+        <v>3.7399999999999998</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>2.8</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
+        <v>383</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>0.83</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>1.07</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.86</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>1.04</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <v>228</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.2199999999999999E-3</v>
+      </c>
+      <c r="E7" s="6">
+        <f>D7*1000</f>
+        <v>1.22</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.2899999999999999E-3</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="1"/>
+        <v>2.29</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.07</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="2">
+        <v>156</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="5">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.91E-3</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
+        <v>1.91</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0600000000000003</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="2">
+        <v>270</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8.8999999999999995E-4</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="1"/>
+        <v>2.85</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.96</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="2">
+        <v>148</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="5">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.9400000000000001E-3</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9400000000000002</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="10">
+        <v>1.5226666666666699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="2">
+        <v>188</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.06E-3</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.06</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4399999999999995</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="10">
+        <f>_xlfn.STDEV.S(E2:E31)</f>
+        <v>0.16177215423260422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>398</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="5">
+        <v>6.4000000000000005E-4</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3.5599999999999998E-3</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="1"/>
+        <v>3.5599999999999996</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="2"/>
+        <v>2.92</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <v>63</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="5">
+        <v>6.4000000000000005E-4</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2599999999999998</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
+        <v>236</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4.0600000000000002E-3</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="1"/>
+        <v>4.0600000000000005</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3600000000000003</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="10">
+        <f>L11/SQRT(L12)</f>
+        <v>2.953541934980072E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
+        <v>321</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6.0999999999999997E-4</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4.8900000000000002E-3</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="1"/>
+        <v>4.8900000000000006</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>4.28</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="2">
+        <v>121</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="5">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="2">
+        <v>317</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="5">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="0"/>
+        <v>0.83</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.8600000000000001E-3</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="1"/>
+        <v>1.86</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.03</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="11">
+        <f>(L14-L13)/L11</f>
+        <v>-247.0787680998464</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
+        <v>184</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="5">
+        <v>8.8000000000000003E-4</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.8600000000000001E-3</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="1"/>
+        <v>1.86</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="L18" s="10">
+        <f>_xlfn.T.DIST(L17,L16,1)</f>
+        <v>4.7382417621052505E-50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
+        <v>87</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="5">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.89E-3</v>
+      </c>
+      <c r="G19" s="7">
+        <f t="shared" si="1"/>
+        <v>1.89</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="2"/>
+        <v>1.04</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L19" s="11">
+        <f>_xlfn.T.INV(L15,L16)</f>
+        <v>-1.6991270265334986</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="2">
+        <v>254</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="5">
+        <v>8.8000000000000003E-4</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="2"/>
+        <v>1.02</v>
+      </c>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="2">
+        <v>185</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.09E-3</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.4599999999999999E-3</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="1"/>
+        <v>1.46</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.36999999999999988</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="2">
+        <v>395</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="5">
+        <v>8.1999999999999998E-4</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.82</v>
+      </c>
+      <c r="F22" s="1">
+        <v>4.4799999999999996E-3</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="1"/>
+        <v>4.4799999999999995</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="2"/>
+        <v>3.6599999999999997</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="2">
+        <v>357</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="5">
+        <v>8.4000000000000003E-4</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="0"/>
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G23" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="2"/>
+        <v>1.06</v>
+      </c>
+      <c r="K23"/>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="2">
+        <v>107</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="5">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.81E-3</v>
+      </c>
+      <c r="G24" s="7">
+        <f t="shared" si="1"/>
+        <v>1.81</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="2"/>
+        <v>0.96000000000000008</v>
+      </c>
+      <c r="K24"/>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="2">
+        <v>230</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="5">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="0"/>
+        <v>0.83</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1.8699999999999999E-3</v>
+      </c>
+      <c r="G25" s="7">
+        <f t="shared" si="1"/>
+        <v>1.8699999999999999</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0399999999999998</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="2">
+        <v>256</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="5">
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="0"/>
+        <v>0.86</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G26" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="2"/>
+        <v>1.04</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
+        <v>253</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1.89E-3</v>
+      </c>
+      <c r="G27" s="7">
+        <f t="shared" si="1"/>
+        <v>1.89</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
+        <v>275</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" s="5">
+        <v>8.4999999999999995E-4</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G28" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="2"/>
+        <v>1.05</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" s="10">
+        <f>G36</f>
+        <v>2.5880000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
+        <v>294</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="5">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1.9E-3</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="10">
+        <f>G37</f>
+        <v>1.1516626661274234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="2">
+        <v>155</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="5">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2.8800000000000002E-3</v>
+      </c>
+      <c r="G30" s="7">
+        <f t="shared" si="1"/>
+        <v>2.8800000000000003</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="2"/>
+        <v>2.08</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L30" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" s="2">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3.0300000000000001E-3</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="1"/>
+        <v>3.0300000000000002</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7300000000000002</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L31" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="I32"/>
+      <c r="K32" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" s="10">
+        <f>L29/SQRT(L30)</f>
+        <v>0.21026387362484353</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="I33"/>
+      <c r="K33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B34" s="2"/>
+      <c r="C34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="I34"/>
+      <c r="K34" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L34" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="I35"/>
+      <c r="K35" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L35" s="11">
+        <f>(L32-L31)/L29</f>
+        <v>-34.549818533383544</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="14">
+        <f>AVERAGE(E2:E31)</f>
+        <v>0.88433333333333342</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="15">
+        <f>AVERAGE(G2:G31)</f>
+        <v>2.5880000000000005</v>
+      </c>
+      <c r="I36" s="2">
+        <f>AVERAGE(I2:I31)</f>
+        <v>1.7036666666666664</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="L36" s="10">
+        <f>_xlfn.T.DIST(L35,L34,1)</f>
+        <v>2.0395037311147106E-25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="14">
+        <f>_xlfn.STDEV.S(E2:E31)</f>
+        <v>0.16177215423260422</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="15">
+        <f>_xlfn.STDEV.S(G2:G31)</f>
+        <v>1.1516626661274234</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L37" s="11">
+        <f>_xlfn.T.INV(L33,L34)</f>
+        <v>-1.6991270265334986</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="14">
+        <v>30</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="15">
+        <v>30</v>
+      </c>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C39"/>
+      <c r="E39"/>
+      <c r="G39"/>
+      <c r="K39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="1">
+        <f>MIN(E2:E31)</f>
+        <v>0.61</v>
+      </c>
+      <c r="G40" s="1">
+        <f>MIN(G2:G31)</f>
+        <v>1.46</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C41" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 1)</f>
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="G41" s="1">
+        <f>_xlfn.QUARTILE.INC(G2:G31, 1)</f>
+        <v>1.8924999999999998</v>
+      </c>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 2)</f>
+        <v>0.85</v>
+      </c>
+      <c r="G42" s="1">
+        <f>_xlfn.QUARTILE.INC(G2:G31, 2)</f>
+        <v>1.9</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 3)</f>
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="G43" s="1">
+        <f>_xlfn.QUARTILE.INC(G2:G31, 3)</f>
+        <v>2.9925000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C44" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" s="1">
+        <f>MAX(E2:E31)</f>
+        <v>1.3</v>
+      </c>
+      <c r="G44" s="1">
+        <f>MAX(G2:G31)</f>
+        <v>5.8999999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C45"/>
+      <c r="E45"/>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C46"/>
+      <c r="E46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C47" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="1">
+        <f>E41-E40</f>
+        <v>0.21250000000000002</v>
+      </c>
+      <c r="G47" s="1">
+        <f>G41-G40</f>
+        <v>0.43249999999999988</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C48" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" s="1">
+        <f>E42-E41</f>
+        <v>2.7499999999999969E-2</v>
+      </c>
+      <c r="G48" s="1">
+        <f>G42-G41</f>
+        <v>7.5000000000000622E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C49" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" s="1">
+        <f>E43-E42</f>
+        <v>4.7499999999999987E-2</v>
+      </c>
+      <c r="G49" s="1">
+        <f>G43-G42</f>
+        <v>1.0925000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="1">
+        <f>E44-E43</f>
+        <v>0.40250000000000008</v>
+      </c>
+      <c r="G50" s="1">
+        <f>G44-G43</f>
+        <v>2.9074999999999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EEE59C-7AEA-4A4E-B2DB-2A83C9882BEF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Latency tests on 30k done
</commit_message>
<xml_diff>
--- a/documentation/figures/latencies.xlsx
+++ b/documentation/figures/latencies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\PSHS 2019\5\R2_B09_Chord_Identification\documentation\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C143FEFB-70CF-4C97-B088-C1466558AE78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD369739-743C-41B8-917E-D548269B1ED0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="989" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="989" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="NNtime" sheetId="4" r:id="rId4"/>
     <sheet name="Totaltime" sheetId="5" r:id="rId5"/>
     <sheet name="6_NN2_4000" sheetId="7" r:id="rId6"/>
-    <sheet name="A" sheetId="6" r:id="rId7"/>
+    <sheet name="6_NN2_30K" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="228">
   <si>
     <t>R2-B09</t>
   </si>
@@ -577,6 +577,144 @@
   </si>
   <si>
     <t>HA: m &lt; 40</t>
+  </si>
+  <si>
+    <t>Eaug</t>
+  </si>
+  <si>
+    <t>CM7sus2</t>
+  </si>
+  <si>
+    <t>A#7sus4</t>
+  </si>
+  <si>
+    <t>F#o7</t>
+  </si>
+  <si>
+    <t>E9sus2</t>
+  </si>
+  <si>
+    <t>Co7</t>
+  </si>
+  <si>
+    <t>Bsus2</t>
+  </si>
+  <si>
+    <t>F#M11</t>
+  </si>
+  <si>
+    <t>D#7</t>
+  </si>
+  <si>
+    <t>A11sus2</t>
+  </si>
+  <si>
+    <t>Dmin</t>
+  </si>
+  <si>
+    <t>A#mM7(9)</t>
+  </si>
+  <si>
+    <t>A#m11</t>
+  </si>
+  <si>
+    <t>Baug</t>
+  </si>
+  <si>
+    <t>Cm6</t>
+  </si>
+  <si>
+    <t>G#M9sus4</t>
+  </si>
+  <si>
+    <t>CM6(9)</t>
+  </si>
+  <si>
+    <t>C#M6(9)</t>
+  </si>
+  <si>
+    <t>F#dim9</t>
+  </si>
+  <si>
+    <t>Dm6(9)</t>
+  </si>
+  <si>
+    <t>A#aug7</t>
+  </si>
+  <si>
+    <t>C#11</t>
+  </si>
+  <si>
+    <t>A9sus4</t>
+  </si>
+  <si>
+    <t>Ddim7</t>
+  </si>
+  <si>
+    <t>Adim9</t>
+  </si>
+  <si>
+    <t>AM7sus2</t>
+  </si>
+  <si>
+    <t>C#7sus2</t>
+  </si>
+  <si>
+    <t>G#M6(9)</t>
+  </si>
+  <si>
+    <t>D#M11sus2</t>
+  </si>
+  <si>
+    <t>C#M9sus4</t>
+  </si>
+  <si>
+    <t>C#m7</t>
+  </si>
+  <si>
+    <t>A#M7</t>
+  </si>
+  <si>
+    <t>EM11</t>
+  </si>
+  <si>
+    <t>Gm7</t>
+  </si>
+  <si>
+    <t>Fdim7</t>
+  </si>
+  <si>
+    <t>GmM7</t>
+  </si>
+  <si>
+    <t>Bo7</t>
+  </si>
+  <si>
+    <t>C#M9</t>
+  </si>
+  <si>
+    <t>D#9sus2</t>
+  </si>
+  <si>
+    <t>F#M9sus2</t>
+  </si>
+  <si>
+    <t>A#11sus2</t>
+  </si>
+  <si>
+    <t>Amin</t>
+  </si>
+  <si>
+    <t>F#M11sus2</t>
+  </si>
+  <si>
+    <t>E7sus2</t>
+  </si>
+  <si>
+    <t>D#mM7</t>
+  </si>
+  <si>
+    <t>B9sus4</t>
   </si>
 </sst>
 </file>
@@ -637,7 +775,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +792,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFFF"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -704,7 +848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -731,6 +875,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,6 +949,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFCCFFCC"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1773,6 +1921,488 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:rPr>
+              <a:t>Neural network response times</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_30K'!$E$46,'6_NN2_30K'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_30K'!$E$47,'6_NN2_30K'!$G$47)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.8799999999999946E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2194999999999974E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF24-4A69-8D0C-5BA4F11C9151}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_30K'!$E$46,'6_NN2_30K'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_30K'!$E$48,'6_NN2_30K'!$G$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.78000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30759000000000014</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF24-4A69-8D0C-5BA4F11C9151}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="A5A5A5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_30K'!$E$46,'6_NN2_30K'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_30K'!$E$49,'6_NN2_30K'!$G$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.13542499999999991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3720799999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FF24-4A69-8D0C-5BA4F11C9151}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>('6_NN2_30K'!$E$46,'6_NN2_30K'!$G$46)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Neural net</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neural net + Translator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('6_NN2_30K'!$E$50,'6_NN2_30K'!$G$50)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>58.101374999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.686295000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FF24-4A69-8D0C-5BA4F11C9151}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="10204729"/>
+        <c:axId val="95714024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="10204729"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95714024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95714024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="HK Grotesk"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="10204729"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1835,6 +2465,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56469778-E25B-4E54-8527-71879B61B600}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1086840</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1072089</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F89E81D-7D1C-4B02-911B-6A5E5FA2BA79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4581,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96F28FD-0BBF-4F5B-9859-054629604D05}">
   <dimension ref="A1:AMK50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -5945,15 +6618,1368 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EEE59C-7AEA-4A4E-B2DB-2A83C9882BEF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A00A45-F8A6-4285-B79B-39CBE7E25130}">
+  <dimension ref="A1:AMK50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.23046875" style="1"/>
+    <col min="2" max="2" width="15.84375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.61328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.53515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.69140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.23046875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.69140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.23046875" style="1"/>
+    <col min="11" max="11" width="17.3046875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.61328125" style="1" customWidth="1"/>
+    <col min="13" max="1025" width="9.23046875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1"/>
+      <c r="L1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
+        <v>151</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5.8966299999999999E-2</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:E31" si="0">D2*1000</f>
+        <v>58.966299999999997</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5.909727E-2</v>
+      </c>
+      <c r="G2" s="7">
+        <f t="shared" ref="G2:G31" si="1">F2*1000</f>
+        <v>59.097270000000002</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I31" si="2">1000*(F2-D2)</f>
+        <v>0.13097000000000109</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
+        <v>13</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8.5729999999999997E-4</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85729999999999995</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.40164E-3</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" si="1"/>
+        <v>1.40164</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="2"/>
+        <v>0.54434000000000005</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="2">
+        <v>386</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8.6260000000000004E-4</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.86260000000000003</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.3754800000000001E-3</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="1"/>
+        <v>3.37548</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>2.5128800000000004</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.1295000000000001E-3</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1295000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.23004E-3</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>1.23004</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10053999999999988</v>
+      </c>
+      <c r="K5"/>
+      <c r="L5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
+        <v>234</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6.7120000000000005E-4</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.67120000000000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.7032600000000001E-3</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="1"/>
+        <v>1.70326</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>1.03206</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <v>303</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.6579999999999997E-4</v>
+      </c>
+      <c r="E7" s="6">
+        <f>D7*1000</f>
+        <v>0.76579999999999993</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3.82263E-3</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="1"/>
+        <v>3.8226300000000002</v>
+      </c>
+      <c r="I7" s="1">
+        <f>1000*(F7-D7)</f>
+        <v>3.0568300000000002</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="2">
+        <v>172</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="5">
+        <v>6.2089999999999997E-4</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7.1308000000000005E-4</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.71308000000000005</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>9.2180000000000081E-2</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="2">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8.0610000000000002E-4</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.80610000000000004</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3.28518E-3</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="1"/>
+        <v>3.28518</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4790799999999997</v>
+      </c>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="2">
+        <v>412</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2.50651E-2</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>25.065100000000001</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.5174289999999998E-2</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="1"/>
+        <v>25.174289999999999</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10918999999999859</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="10">
+        <v>1.5226666666666699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="2">
+        <v>248</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="5">
+        <v>6.2239999999999995E-4</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.62239999999999995</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7.1277000000000005E-4</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.71277000000000001</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="2"/>
+        <v>9.0370000000000103E-2</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="10">
+        <f>_xlfn.STDEV.S(E2:E31)</f>
+        <v>12.005527192713716</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>120</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7.4529999999999996E-4</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.74529999999999996</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.5724099999999998E-3</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="1"/>
+        <v>2.5724099999999996</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8271099999999998</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <v>364</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="5">
+        <v>6.0289999999999996E-4</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.60289999999999999</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6.9910999999999997E-4</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.69911000000000001</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>9.6210000000000004E-2</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
+        <v>76</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2.49506E-2</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>24.950600000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.5055129999999998E-2</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="1"/>
+        <v>25.055129999999998</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10452999999999851</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="10">
+        <f>L11/SQRT(L12)</f>
+        <v>2.1918993527303248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
+        <v>403</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6.4139999999999998E-4</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64139999999999997</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7.3014E-4</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="1"/>
+        <v>0.73014000000000001</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>8.8740000000000027E-2</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="2">
+        <v>397</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="5">
+        <v>6.2859999999999999E-4</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="0"/>
+        <v>0.62860000000000005</v>
+      </c>
+      <c r="F16" s="1">
+        <v>7.1958999999999999E-4</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.71958999999999995</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="2"/>
+        <v>9.0989999999999988E-2</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="2">
+        <v>410</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1.8249E-3</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8249</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.9266699999999999E-3</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9266699999999999</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10176999999999994</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="11">
+        <f>(L14-L13)/L11</f>
+        <v>-3.1492245230360081</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D18" s="5">
+        <v>7.6769000000000004E-3</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="0"/>
+        <v>7.6769000000000007</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3.8400000000000001E-3</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="1"/>
+        <v>3.8400000000000003</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>-3.8369000000000004</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="L18" s="10">
+        <f>_xlfn.T.DIST(L17,L16,1)</f>
+        <v>1.8883282941076626E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
+        <v>134</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="5">
+        <v>7.0719999999999995E-4</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="0"/>
+        <v>0.70719999999999994</v>
+      </c>
+      <c r="F19" s="1">
+        <v>7.9841000000000005E-4</v>
+      </c>
+      <c r="G19" s="7">
+        <f t="shared" si="1"/>
+        <v>0.79841000000000006</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="2"/>
+        <v>9.1210000000000097E-2</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L19" s="11">
+        <f>_xlfn.T.INV(L15,L16)</f>
+        <v>-1.6991270265334986</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="2">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="5">
+        <v>6.4260000000000001E-4</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64260000000000006</v>
+      </c>
+      <c r="F20" s="1">
+        <v>7.2827999999999999E-4</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="1"/>
+        <v>0.72828000000000004</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="2"/>
+        <v>8.5679999999999978E-2</v>
+      </c>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="2">
+        <v>272</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D21" s="5">
+        <v>6.7549999999999999E-4</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.67549999999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <v>8.3967999999999998E-4</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="1"/>
+        <v>0.83967999999999998</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.16417999999999999</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="2">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="5">
+        <v>6.3270000000000004E-4</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="0"/>
+        <v>0.63270000000000004</v>
+      </c>
+      <c r="F22" s="1">
+        <v>7.2610999999999997E-4</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="1"/>
+        <v>0.72610999999999992</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="2"/>
+        <v>9.3409999999999938E-2</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="2">
+        <v>243</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D23" s="5">
+        <v>6.3820000000000001E-4</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="0"/>
+        <v>0.63819999999999999</v>
+      </c>
+      <c r="F23" s="1">
+        <v>7.3200999999999995E-4</v>
+      </c>
+      <c r="G23" s="7">
+        <f t="shared" si="1"/>
+        <v>0.73200999999999994</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="2"/>
+        <v>9.3809999999999949E-2</v>
+      </c>
+      <c r="K23"/>
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="2">
+        <v>111</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="D24" s="5">
+        <v>6.6929999999999995E-4</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="0"/>
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7.7481999999999996E-4</v>
+      </c>
+      <c r="G24" s="7">
+        <f t="shared" si="1"/>
+        <v>0.77481999999999995</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10552</v>
+      </c>
+      <c r="K24"/>
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="2">
+        <v>380</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" s="5">
+        <v>8.6569999999999995E-4</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="0"/>
+        <v>0.86569999999999991</v>
+      </c>
+      <c r="F25" s="1">
+        <v>9.5945999999999998E-4</v>
+      </c>
+      <c r="G25" s="7">
+        <f t="shared" si="1"/>
+        <v>0.95945999999999998</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="2"/>
+        <v>9.3760000000000024E-2</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="2">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="5">
+        <v>7.4910000000000005E-4</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="0"/>
+        <v>0.7491000000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>8.3998999999999999E-4</v>
+      </c>
+      <c r="G26" s="7">
+        <f t="shared" si="1"/>
+        <v>0.83999000000000001</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="2"/>
+        <v>9.0889999999999943E-2</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
+        <v>358</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="5">
+        <v>6.3920000000000003E-4</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="0"/>
+        <v>0.63919999999999999</v>
+      </c>
+      <c r="F27" s="1">
+        <v>7.3107000000000001E-4</v>
+      </c>
+      <c r="G27" s="7">
+        <f t="shared" si="1"/>
+        <v>0.73107</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="2"/>
+        <v>9.1869999999999979E-2</v>
+      </c>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
+        <v>85</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="5">
+        <v>7.8910000000000004E-4</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="0"/>
+        <v>0.78910000000000002</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1.1288800000000001E-3</v>
+      </c>
+      <c r="G28" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1288800000000001</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33978000000000003</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L28" s="10">
+        <f>G36</f>
+        <v>4.9371113333333341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
+        <v>354</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1.0053E-3</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0053000000000001</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1.1183300000000001E-3</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="1"/>
+        <v>1.11833</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="2"/>
+        <v>0.11303000000000007</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="10">
+        <f>G37</f>
+        <v>11.899028509812434</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="2">
+        <v>346</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="5">
+        <v>6.6719999999999995E-4</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="0"/>
+        <v>0.6671999999999999</v>
+      </c>
+      <c r="F30" s="1">
+        <v>7.6241999999999998E-4</v>
+      </c>
+      <c r="G30" s="7">
+        <f t="shared" si="1"/>
+        <v>0.76241999999999999</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="2"/>
+        <v>9.5220000000000027E-2</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L30" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" s="2">
+        <v>52</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D31" s="5">
+        <v>7.1369999999999995E-4</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="0"/>
+        <v>0.7137</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1.91519E-3</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9151899999999999</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2014899999999999</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="L31" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="I32"/>
+      <c r="K32" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" s="10">
+        <f>L29/SQRT(L30)</f>
+        <v>2.1724554424071174</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="I33"/>
+      <c r="K33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33" s="10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B34" s="2"/>
+      <c r="C34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="I34"/>
+      <c r="K34" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L34" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="I35"/>
+      <c r="K35" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L35" s="11">
+        <f>(L32-L31)/L29</f>
+        <v>-3.1790447872613057</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="14">
+        <f>AVERAGE(E2:E31)</f>
+        <v>4.5610866666666663</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="15">
+        <f>AVERAGE(G2:G31)</f>
+        <v>4.9371113333333341</v>
+      </c>
+      <c r="I36" s="2">
+        <f>AVERAGE(I2:I31)</f>
+        <v>0.37602466666666656</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="L36" s="10">
+        <f>_xlfn.T.DIST(L35,L34,1)</f>
+        <v>1.7503513843093613E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="14">
+        <f>_xlfn.STDEV.S(E2:E31)</f>
+        <v>12.005527192713716</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="15">
+        <f>_xlfn.STDEV.S(G2:G31)</f>
+        <v>11.899028509812434</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L37" s="11">
+        <f>_xlfn.T.INV(L33,L34)</f>
+        <v>-1.6991270265334986</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="15.45" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="14">
+        <v>30</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="15">
+        <v>30</v>
+      </c>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C39"/>
+      <c r="E39"/>
+      <c r="G39"/>
+      <c r="K39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="1">
+        <f>MIN(E2:E31)</f>
+        <v>0.60289999999999999</v>
+      </c>
+      <c r="G40" s="1">
+        <f>MIN(G2:G31)</f>
+        <v>0.69911000000000001</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C41" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 1)</f>
+        <v>0.64169999999999994</v>
+      </c>
+      <c r="G41" s="1">
+        <f>_xlfn.QUARTILE.INC(G2:G31, 1)</f>
+        <v>0.73130499999999998</v>
+      </c>
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 2)</f>
+        <v>0.72950000000000004</v>
+      </c>
+      <c r="G42" s="1">
+        <f>_xlfn.QUARTILE.INC(G2:G31, 2)</f>
+        <v>1.0388950000000001</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="1">
+        <f>_xlfn.QUARTILE.INC(E2:E31, 3)</f>
+        <v>0.86492499999999994</v>
+      </c>
+      <c r="G43" s="1">
+        <f>_xlfn.QUARTILE.INC(G2:G31, 3)</f>
+        <v>2.4109749999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C44" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" s="1">
+        <f>MAX(E2:E31)</f>
+        <v>58.966299999999997</v>
+      </c>
+      <c r="G44" s="1">
+        <f>MAX(G2:G31)</f>
+        <v>59.097270000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C45"/>
+      <c r="E45"/>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C46"/>
+      <c r="E46" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C47" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="1">
+        <f>E41-E40</f>
+        <v>3.8799999999999946E-2</v>
+      </c>
+      <c r="G47" s="1">
+        <f>G41-G40</f>
+        <v>3.2194999999999974E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="C48" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E48" s="1">
+        <f>E42-E41</f>
+        <v>8.78000000000001E-2</v>
+      </c>
+      <c r="G48" s="1">
+        <f>G42-G41</f>
+        <v>0.30759000000000014</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C49" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" s="1">
+        <f>E43-E42</f>
+        <v>0.13542499999999991</v>
+      </c>
+      <c r="G49" s="1">
+        <f>G43-G42</f>
+        <v>1.3720799999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="C50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="1">
+        <f>E44-E43</f>
+        <v>58.101374999999997</v>
+      </c>
+      <c r="G50" s="1">
+        <f>G44-G43</f>
+        <v>56.686295000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>